<commit_message>
metFile for generate can have extra #columns not mapped to components
</commit_message>
<xml_diff>
--- a/examples/library_def.xlsx
+++ b/examples/library_def.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>display_id</t>
   </si>
@@ -42,15 +42,6 @@
     <t>sll0558</t>
   </si>
   <si>
-    <t>cs0002_{key}</t>
-  </si>
-  <si>
-    <t>cs0003_{key}</t>
-  </si>
-  <si>
-    <t>cs0004_{key}</t>
-  </si>
-  <si>
     <t>author</t>
   </si>
   <si>
@@ -94,6 +85,18 @@
   </si>
   <si>
     <t>CCAATTGA</t>
+  </si>
+  <si>
+    <t>#pref</t>
+  </si>
+  <si>
+    <t>cs0002</t>
+  </si>
+  <si>
+    <t>cs0003</t>
+  </si>
+  <si>
+    <t>cs0004</t>
   </si>
 </sst>
 </file>
@@ -411,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -419,111 +422,131 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE(A2,"_","{key}")</f>
+        <v>cs0002_{key}</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C4" si="0">CONCATENATE(A3,"_","{key}")</f>
+        <v>cs0003_{key}</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>cs0004_{key}</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
         <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>